<commit_message>
defect report added to air wallex project submission
</commit_message>
<xml_diff>
--- a/Defect Sheet.xlsx
+++ b/Defect Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chackom/Desktop/AirWallexAutomationTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B9DA60-3080-4A41-8AD9-25ADCBEC8942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86223444-EB61-694D-A3F3-F2CB914F59C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{3839D7BE-AF48-F148-8D99-3AAE2C097819}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>SlNo</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>BSB number accepts all alphabets , even if no numbers are given, no particular error message.</t>
+  </si>
+  <si>
+    <t>Non functional</t>
+  </si>
+  <si>
+    <t>Performace,Compliance testing should als be done on this.</t>
   </si>
 </sst>
 </file>
@@ -767,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D14882-11BA-7141-A8B1-2EC38BDA6ABB}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,37 +950,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>